<commit_message>
Add Pie Graph for Playbook Metrics
Add a pie chart to output the total minutes per process step (total).
</commit_message>
<xml_diff>
--- a/python--deployment-metric-parser/examples/Playbook_2.xlsx
+++ b/python--deployment-metric-parser/examples/Playbook_2.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="2240" windowWidth="33000" windowHeight="14540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4780" yWindow="5180" windowWidth="33000" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="Playbook" sheetId="1" r:id="rId2"/>
-    <sheet name="Task States" sheetId="3" r:id="rId3"/>
+    <sheet name="Meta" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
   <si>
     <t>Step</t>
   </si>
@@ -243,6 +243,21 @@
   </si>
   <si>
     <t>3:30pm</t>
+  </si>
+  <si>
+    <t>Task States</t>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Estimated Start Date</t>
+  </si>
+  <si>
+    <t>Actual Start Date</t>
   </si>
 </sst>
 </file>
@@ -292,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -329,6 +344,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,7 +657,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="10">
-        <v>43108</v>
+        <v>43107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -750,28 +766,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="22" style="5" customWidth="1"/>
-    <col min="11" max="11" width="38.6640625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="44" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="17.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="22" style="5" customWidth="1"/>
+    <col min="13" max="13" width="38.6640625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -781,35 +798,41 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -819,28 +842,34 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14">
+        <v>42742</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="14">
+        <v>43108</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -850,29 +879,35 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="14">
+        <v>42742</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5">
+      <c r="I3" s="14">
+        <v>43108</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="5">
         <v>15</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="9"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -882,27 +917,33 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="14">
+        <v>42742</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="14">
+        <v>43108</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="9"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -912,27 +953,33 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="14">
+        <v>42742</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="14">
+        <v>43108</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -942,30 +989,36 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14">
+        <v>42742</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="14">
+        <v>43108</v>
+      </c>
+      <c r="J6" s="6">
         <v>0.56041666666666667</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -975,73 +1028,79 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="14">
+        <v>42742</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="14">
+        <v>43108</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L16" s="9"/>
-    </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L17" s="9"/>
-    </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L19" s="9"/>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L20" s="9"/>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L21" s="9"/>
-    </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L22" s="9"/>
-    </row>
-    <row r="23" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L23" s="9"/>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N22" s="9"/>
+    </row>
+    <row r="23" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1050,9 +1109,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Task States'!$A$1:$A$4</xm:f>
+            <xm:f>Meta!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G996</xm:sqref>
+          <xm:sqref>H2:H996 I8:I996</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1062,29 +1121,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>